<commit_message>
Changes at 01 Analyse and 02 Zeitplanung
</commit_message>
<xml_diff>
--- a/documents/02 Zeitplanung.xlsx
+++ b/documents/02 Zeitplanung.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Ist Arbeitszeit - Übersicht" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'IPA Zeitplanung'!$A$1:$AC$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'IPA Zeitplanung'!$A$1:$AC$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Ist Arbeitszeit - Übersicht'!$A$1:$O$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Nr.</t>
   </si>
@@ -282,6 +282,21 @@
   </si>
   <si>
     <t>Ferien</t>
+  </si>
+  <si>
+    <t>F.REQ.007</t>
+  </si>
+  <si>
+    <t>F.REQ.008</t>
+  </si>
+  <si>
+    <t>F.REQ.009</t>
+  </si>
+  <si>
+    <t>F.REQ.010</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +497,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="77">
     <border>
@@ -1435,7 +1474,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1907,12 +1946,6 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1966,6 +1999,30 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="73" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
@@ -2307,19 +2364,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2384,7 +2441,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>14</c:v>
@@ -2900,13 +2957,13 @@
   <sheetPr codeName="Tabelle1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AM38"/>
+  <dimension ref="A1:AM42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2926,37 +2983,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="170"/>
-      <c r="T1" s="170"/>
-      <c r="U1" s="170"/>
-      <c r="V1" s="170"/>
-      <c r="W1" s="170"/>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="170"/>
-      <c r="Z1" s="170"/>
-      <c r="AA1" s="170"/>
-      <c r="AB1" s="170"/>
-      <c r="AC1" s="170"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="168"/>
+      <c r="W1" s="168"/>
+      <c r="X1" s="168"/>
+      <c r="Y1" s="168"/>
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="168"/>
+      <c r="AB1" s="168"/>
+      <c r="AC1" s="168"/>
     </row>
     <row r="2" spans="1:33" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
@@ -2972,43 +3029,43 @@
     <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="69"/>
       <c r="B3" s="73"/>
-      <c r="C3" s="172" t="s">
+      <c r="C3" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="172"/>
+      <c r="D3" s="170"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="172" t="s">
+      <c r="J3" s="170" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="172"/>
-      <c r="L3" s="172"/>
-      <c r="M3" s="172"/>
-      <c r="N3" s="174"/>
-      <c r="O3" s="171" t="s">
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="172"/>
+      <c r="O3" s="169" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="172"/>
-      <c r="Q3" s="172"/>
-      <c r="R3" s="172"/>
-      <c r="S3" s="172"/>
-      <c r="T3" s="171" t="s">
+      <c r="P3" s="170"/>
+      <c r="Q3" s="170"/>
+      <c r="R3" s="170"/>
+      <c r="S3" s="170"/>
+      <c r="T3" s="169" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="172"/>
-      <c r="V3" s="172"/>
-      <c r="W3" s="172"/>
-      <c r="X3" s="172"/>
-      <c r="Y3" s="171" t="s">
+      <c r="U3" s="170"/>
+      <c r="V3" s="170"/>
+      <c r="W3" s="170"/>
+      <c r="X3" s="170"/>
+      <c r="Y3" s="169" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="172"/>
-      <c r="AA3" s="172"/>
-      <c r="AB3" s="172"/>
-      <c r="AC3" s="173"/>
+      <c r="Z3" s="170"/>
+      <c r="AA3" s="170"/>
+      <c r="AB3" s="170"/>
+      <c r="AC3" s="171"/>
       <c r="AD3" s="13"/>
       <c r="AE3" s="13"/>
       <c r="AF3" s="13"/>
@@ -3067,11 +3124,11 @@
         <f>P4+1</f>
         <v>42711</v>
       </c>
-      <c r="R4" s="164">
+      <c r="R4" s="162">
         <f>Q4+1</f>
         <v>42712</v>
       </c>
-      <c r="S4" s="164">
+      <c r="S4" s="162">
         <f>R4+1</f>
         <v>42713</v>
       </c>
@@ -3125,7 +3182,7 @@
       </c>
       <c r="C5" s="93">
         <f>SUM(C6:C10)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="94">
         <f>SUM(D6:D10)</f>
@@ -3175,7 +3232,7 @@
       <c r="G6" s="61"/>
       <c r="H6" s="37"/>
       <c r="I6" s="86" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="J6" s="122"/>
       <c r="K6" s="39"/>
@@ -3262,7 +3319,9 @@
       <c r="F8" s="35"/>
       <c r="G8" s="61"/>
       <c r="H8" s="37"/>
-      <c r="I8" s="87"/>
+      <c r="I8" s="87" t="s">
+        <v>37</v>
+      </c>
       <c r="J8" s="122"/>
       <c r="K8" s="123"/>
       <c r="L8" s="135"/>
@@ -3295,7 +3354,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="36" t="str">
         <f t="shared" si="0"/>
@@ -3312,7 +3371,7 @@
       <c r="K9" s="39"/>
       <c r="L9" s="47"/>
       <c r="M9" s="47"/>
-      <c r="N9" s="62"/>
+      <c r="N9" s="136"/>
       <c r="O9" s="48"/>
       <c r="P9" s="49"/>
       <c r="Q9" s="39"/>
@@ -3384,7 +3443,7 @@
       </c>
       <c r="D11" s="93">
         <f>SUM(D12:D14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="95"/>
       <c r="F11" s="96"/>
@@ -3423,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="35"/>
@@ -3537,8 +3596,8 @@
         <v>11</v>
       </c>
       <c r="C15" s="93">
-        <f>SUM(C16:C21)</f>
-        <v>36</v>
+        <f>SUM(C16:C29)</f>
+        <v>152</v>
       </c>
       <c r="D15" s="94">
         <f>SUM(D16:D21)</f>
@@ -3578,7 +3637,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" s="60">
         <v>8</v>
@@ -3589,11 +3648,13 @@
       <c r="F16" s="35"/>
       <c r="G16" s="61"/>
       <c r="H16" s="37"/>
-      <c r="I16" s="87"/>
+      <c r="I16" s="87" t="s">
+        <v>53</v>
+      </c>
       <c r="J16" s="61"/>
       <c r="K16" s="39"/>
       <c r="L16" s="39"/>
-      <c r="M16" s="163"/>
+      <c r="M16" s="161"/>
       <c r="N16" s="150"/>
       <c r="O16" s="151"/>
       <c r="P16" s="152"/>
@@ -3619,23 +3680,25 @@
         <v>39</v>
       </c>
       <c r="C17" s="35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D17" s="60">
         <v>6</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="183">
         <v>1</v>
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="61"/>
       <c r="H17" s="37"/>
-      <c r="I17" s="87"/>
+      <c r="I17" s="87" t="s">
+        <v>53</v>
+      </c>
       <c r="J17" s="61"/>
       <c r="K17" s="39"/>
       <c r="L17" s="39"/>
       <c r="M17" s="123"/>
-      <c r="N17" s="136"/>
+      <c r="N17" s="150"/>
       <c r="O17" s="151"/>
       <c r="P17" s="152"/>
       <c r="Q17" s="149"/>
@@ -3660,22 +3723,24 @@
         <v>40</v>
       </c>
       <c r="C18" s="35">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D18" s="60"/>
-      <c r="E18" s="34">
+      <c r="E18" s="183">
         <v>1</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="61"/>
       <c r="H18" s="37"/>
-      <c r="I18" s="87"/>
+      <c r="I18" s="87" t="s">
+        <v>37</v>
+      </c>
       <c r="J18" s="61"/>
       <c r="K18" s="39"/>
       <c r="L18" s="39"/>
       <c r="M18" s="149"/>
       <c r="N18" s="136"/>
-      <c r="O18" s="145"/>
+      <c r="O18" s="151"/>
       <c r="P18" s="152"/>
       <c r="Q18" s="149"/>
       <c r="R18" s="152"/>
@@ -3699,10 +3764,10 @@
         <v>41</v>
       </c>
       <c r="C19" s="35">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D19" s="60"/>
-      <c r="E19" s="34">
+      <c r="E19" s="183">
         <v>1</v>
       </c>
       <c r="F19" s="35"/>
@@ -3717,7 +3782,7 @@
       <c r="O19" s="145"/>
       <c r="P19" s="152"/>
       <c r="Q19" s="149"/>
-      <c r="R19" s="146"/>
+      <c r="R19" s="152"/>
       <c r="S19" s="153"/>
       <c r="T19" s="154"/>
       <c r="U19" s="149"/>
@@ -3738,10 +3803,10 @@
         <v>42</v>
       </c>
       <c r="C20" s="35">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D20" s="60"/>
-      <c r="E20" s="34">
+      <c r="E20" s="183">
         <v>1</v>
       </c>
       <c r="F20" s="35"/>
@@ -3754,9 +3819,9 @@
       <c r="M20" s="149"/>
       <c r="N20" s="150"/>
       <c r="O20" s="145"/>
-      <c r="P20" s="152"/>
+      <c r="P20" s="146"/>
       <c r="Q20" s="149"/>
-      <c r="R20" s="146"/>
+      <c r="R20" s="152"/>
       <c r="S20" s="153"/>
       <c r="T20" s="154"/>
       <c r="U20" s="149"/>
@@ -3777,14 +3842,14 @@
         <v>43</v>
       </c>
       <c r="C21" s="45">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D21" s="36" t="str">
         <f>IF(SUM(J21:AC21)=0," ",SUM(J21:AC21))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E21" s="44">
-        <v>3</v>
+      <c r="E21" s="184">
+        <v>1</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="61"/>
@@ -3796,17 +3861,17 @@
       <c r="M21" s="156"/>
       <c r="N21" s="150"/>
       <c r="O21" s="157"/>
-      <c r="P21" s="158"/>
+      <c r="P21" s="138"/>
       <c r="Q21" s="149"/>
       <c r="R21" s="158"/>
       <c r="S21" s="159"/>
       <c r="T21" s="143"/>
       <c r="U21" s="156"/>
-      <c r="V21" s="149"/>
-      <c r="W21" s="135"/>
-      <c r="X21" s="161"/>
-      <c r="Y21" s="162"/>
-      <c r="Z21" s="158"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="45"/>
+      <c r="Y21" s="180"/>
+      <c r="Z21" s="49"/>
       <c r="AA21" s="49"/>
       <c r="AB21" s="36"/>
       <c r="AC21" s="80"/>
@@ -3816,17 +3881,14 @@
         <v>37</v>
       </c>
       <c r="B22" s="83" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C22" s="45">
-        <v>9</v>
-      </c>
-      <c r="D22" s="36" t="str">
-        <f t="shared" ref="D22:D25" si="2">IF(SUM(J22:AC22)=0," ",SUM(J22:AC22))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E22" s="44">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="182">
+        <v>2</v>
       </c>
       <c r="F22" s="35"/>
       <c r="G22" s="61"/>
@@ -3835,20 +3897,20 @@
       <c r="J22" s="54"/>
       <c r="K22" s="47"/>
       <c r="L22" s="47"/>
-      <c r="M22" s="156"/>
-      <c r="N22" s="150"/>
-      <c r="O22" s="157"/>
-      <c r="P22" s="158"/>
-      <c r="Q22" s="149"/>
-      <c r="R22" s="158"/>
-      <c r="S22" s="159"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="50"/>
       <c r="T22" s="143"/>
-      <c r="U22" s="156"/>
-      <c r="V22" s="149"/>
+      <c r="U22" s="47"/>
+      <c r="V22" s="39"/>
       <c r="W22" s="135"/>
-      <c r="X22" s="147"/>
-      <c r="Y22" s="162"/>
-      <c r="Z22" s="158"/>
+      <c r="X22" s="45"/>
+      <c r="Y22" s="180"/>
+      <c r="Z22" s="49"/>
       <c r="AA22" s="49"/>
       <c r="AB22" s="36"/>
       <c r="AC22" s="80"/>
@@ -3858,17 +3920,14 @@
         <v>38</v>
       </c>
       <c r="B23" s="83" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C23" s="45">
-        <v>7</v>
-      </c>
-      <c r="D23" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E23" s="44">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="182">
+        <v>2</v>
       </c>
       <c r="F23" s="35"/>
       <c r="G23" s="61"/>
@@ -3877,20 +3936,20 @@
       <c r="J23" s="54"/>
       <c r="K23" s="47"/>
       <c r="L23" s="47"/>
-      <c r="M23" s="156"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="157"/>
-      <c r="P23" s="158"/>
-      <c r="Q23" s="149"/>
-      <c r="R23" s="158"/>
-      <c r="S23" s="159"/>
-      <c r="T23" s="160"/>
-      <c r="U23" s="156"/>
-      <c r="V23" s="149"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="143"/>
+      <c r="U23" s="47"/>
+      <c r="V23" s="39"/>
       <c r="W23" s="135"/>
-      <c r="X23" s="147"/>
-      <c r="Y23" s="148"/>
-      <c r="Z23" s="158"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="180"/>
+      <c r="Z23" s="49"/>
       <c r="AA23" s="49"/>
       <c r="AB23" s="36"/>
       <c r="AC23" s="80"/>
@@ -3900,17 +3959,14 @@
         <v>39</v>
       </c>
       <c r="B24" s="83" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C24" s="45">
-        <v>5</v>
-      </c>
-      <c r="D24" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E24" s="44">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="182">
+        <v>2</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="61"/>
@@ -3919,20 +3975,20 @@
       <c r="J24" s="54"/>
       <c r="K24" s="47"/>
       <c r="L24" s="47"/>
-      <c r="M24" s="156"/>
-      <c r="N24" s="150"/>
-      <c r="O24" s="157"/>
-      <c r="P24" s="158"/>
-      <c r="Q24" s="149"/>
-      <c r="R24" s="158"/>
-      <c r="S24" s="159"/>
-      <c r="T24" s="160"/>
-      <c r="U24" s="156"/>
-      <c r="V24" s="149"/>
-      <c r="W24" s="156"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="47"/>
       <c r="X24" s="147"/>
-      <c r="Y24" s="148"/>
-      <c r="Z24" s="158"/>
+      <c r="Y24" s="180"/>
+      <c r="Z24" s="49"/>
       <c r="AA24" s="49"/>
       <c r="AB24" s="36"/>
       <c r="AC24" s="80"/>
@@ -3942,16 +3998,13 @@
         <v>40</v>
       </c>
       <c r="B25" s="83" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C25" s="45">
-        <v>2</v>
-      </c>
-      <c r="D25" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E25" s="44">
+        <v>6</v>
+      </c>
+      <c r="D25" s="36"/>
+      <c r="E25" s="181">
         <v>3</v>
       </c>
       <c r="F25" s="35"/>
@@ -3961,344 +4014,512 @@
       <c r="J25" s="54"/>
       <c r="K25" s="47"/>
       <c r="L25" s="47"/>
-      <c r="M25" s="156"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="157"/>
-      <c r="P25" s="158"/>
-      <c r="Q25" s="149"/>
-      <c r="R25" s="158"/>
-      <c r="S25" s="159"/>
-      <c r="T25" s="160"/>
-      <c r="U25" s="156"/>
-      <c r="V25" s="149"/>
-      <c r="W25" s="156"/>
-      <c r="X25" s="161"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="47"/>
+      <c r="V25" s="39"/>
+      <c r="W25" s="47"/>
+      <c r="X25" s="45"/>
       <c r="Y25" s="148"/>
-      <c r="Z25" s="158"/>
+      <c r="Z25" s="49"/>
       <c r="AA25" s="49"/>
       <c r="AB25" s="36"/>
       <c r="AC25" s="80"/>
     </row>
     <row r="26" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="90">
-        <v>50</v>
-      </c>
-      <c r="B26" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="93">
-        <f>SUM(C27)</f>
-        <v>26</v>
-      </c>
-      <c r="D26" s="94">
-        <f>SUM(D27)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="95"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="99"/>
-      <c r="J26" s="96"/>
-      <c r="K26" s="100"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="102"/>
-      <c r="N26" s="95"/>
-      <c r="O26" s="92"/>
-      <c r="P26" s="101"/>
-      <c r="Q26" s="102"/>
-      <c r="R26" s="100"/>
-      <c r="S26" s="97"/>
-      <c r="T26" s="92"/>
-      <c r="U26" s="101"/>
-      <c r="V26" s="101"/>
-      <c r="W26" s="101"/>
-      <c r="X26" s="97"/>
-      <c r="Y26" s="92"/>
-      <c r="Z26" s="101"/>
-      <c r="AA26" s="101"/>
-      <c r="AB26" s="102"/>
-      <c r="AC26" s="103"/>
+      <c r="A26" s="71">
+        <v>41</v>
+      </c>
+      <c r="B26" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="45">
+        <v>12</v>
+      </c>
+      <c r="D26" s="36" t="str">
+        <f t="shared" ref="D26:D29" si="2">IF(SUM(J26:AC26)=0," ",SUM(J26:AC26))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E26" s="184">
+        <v>1</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="156"/>
+      <c r="N26" s="150"/>
+      <c r="O26" s="157"/>
+      <c r="P26" s="158"/>
+      <c r="Q26" s="149"/>
+      <c r="R26" s="158"/>
+      <c r="S26" s="159"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="156"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="45"/>
+      <c r="Y26" s="186"/>
+      <c r="Z26" s="49"/>
+      <c r="AA26" s="49"/>
+      <c r="AB26" s="143"/>
+      <c r="AC26" s="80"/>
     </row>
     <row r="27" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="72">
-        <v>51</v>
-      </c>
-      <c r="B27" s="84" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="58">
-        <f>SUM(C5,C11,C15)*0.5</f>
-        <v>26</v>
-      </c>
-      <c r="D27" s="66" t="str">
-        <f>IF(SUM(J27:AC27)=0," ",SUM(J27:AC27))</f>
+      <c r="A27" s="71">
+        <v>42</v>
+      </c>
+      <c r="B27" s="83" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="45">
+        <v>12</v>
+      </c>
+      <c r="D27" s="36" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E27" s="63">
-        <v>3</v>
-      </c>
-      <c r="F27" s="58"/>
-      <c r="G27" s="67"/>
+      <c r="E27" s="184">
+        <v>1</v>
+      </c>
+      <c r="F27" s="35"/>
+      <c r="G27" s="61"/>
       <c r="H27" s="37"/>
       <c r="I27" s="87"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="57"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="66"/>
-      <c r="U27" s="57"/>
-      <c r="V27" s="57"/>
-      <c r="W27" s="57"/>
-      <c r="X27" s="59"/>
-      <c r="Y27" s="68"/>
-      <c r="Z27" s="65"/>
-      <c r="AA27" s="65"/>
-      <c r="AB27" s="65"/>
-      <c r="AC27" s="79"/>
-    </row>
-    <row r="28" spans="1:29" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="108" t="s">
+      <c r="J27" s="54"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="156"/>
+      <c r="N27" s="150"/>
+      <c r="O27" s="157"/>
+      <c r="P27" s="158"/>
+      <c r="Q27" s="149"/>
+      <c r="R27" s="158"/>
+      <c r="S27" s="159"/>
+      <c r="T27" s="160"/>
+      <c r="U27" s="156"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="180"/>
+      <c r="Z27" s="49"/>
+      <c r="AA27" s="49"/>
+      <c r="AB27" s="143"/>
+      <c r="AC27" s="134"/>
+    </row>
+    <row r="28" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="71">
+        <v>43</v>
+      </c>
+      <c r="B28" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="45">
+        <v>8</v>
+      </c>
+      <c r="D28" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E28" s="181">
+        <v>3</v>
+      </c>
+      <c r="F28" s="35"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="156"/>
+      <c r="N28" s="150"/>
+      <c r="O28" s="157"/>
+      <c r="P28" s="158"/>
+      <c r="Q28" s="149"/>
+      <c r="R28" s="158"/>
+      <c r="S28" s="159"/>
+      <c r="T28" s="160"/>
+      <c r="U28" s="156"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="47"/>
+      <c r="X28" s="45"/>
+      <c r="Y28" s="180"/>
+      <c r="Z28" s="49"/>
+      <c r="AA28" s="49"/>
+      <c r="AB28" s="185"/>
+      <c r="AC28" s="187"/>
+    </row>
+    <row r="29" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="71">
+        <v>44</v>
+      </c>
+      <c r="B29" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="45">
+        <v>8</v>
+      </c>
+      <c r="D29" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E29" s="181">
+        <v>3</v>
+      </c>
+      <c r="F29" s="35"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="156"/>
+      <c r="N29" s="150"/>
+      <c r="O29" s="157"/>
+      <c r="P29" s="158"/>
+      <c r="Q29" s="149"/>
+      <c r="R29" s="158"/>
+      <c r="S29" s="159"/>
+      <c r="T29" s="160"/>
+      <c r="U29" s="156"/>
+      <c r="V29" s="39"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="180"/>
+      <c r="Z29" s="49"/>
+      <c r="AA29" s="49"/>
+      <c r="AB29" s="185"/>
+      <c r="AC29" s="187"/>
+    </row>
+    <row r="30" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="90">
+        <v>50</v>
+      </c>
+      <c r="B30" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="93">
+        <f>SUM(C31)</f>
+        <v>34</v>
+      </c>
+      <c r="D30" s="94">
+        <f>SUM(D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="95"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="99"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="101"/>
+      <c r="M30" s="102"/>
+      <c r="N30" s="95"/>
+      <c r="O30" s="92"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="102"/>
+      <c r="R30" s="100"/>
+      <c r="S30" s="97"/>
+      <c r="T30" s="92"/>
+      <c r="U30" s="101"/>
+      <c r="V30" s="101"/>
+      <c r="W30" s="101"/>
+      <c r="X30" s="97"/>
+      <c r="Y30" s="92"/>
+      <c r="Z30" s="101"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="102"/>
+      <c r="AC30" s="103"/>
+    </row>
+    <row r="31" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="72">
+        <v>51</v>
+      </c>
+      <c r="B31" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="58">
+        <f>SUM(C5,C11,C15)*0.2</f>
+        <v>34</v>
+      </c>
+      <c r="D31" s="66" t="str">
+        <f>IF(SUM(J31:AC31)=0," ",SUM(J31:AC31))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E31" s="63">
+        <v>3</v>
+      </c>
+      <c r="F31" s="58"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="87"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="65"/>
+      <c r="S31" s="53"/>
+      <c r="T31" s="66"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="59"/>
+      <c r="Y31" s="68"/>
+      <c r="Z31" s="65"/>
+      <c r="AA31" s="65"/>
+      <c r="AB31" s="65"/>
+      <c r="AC31" s="79"/>
+    </row>
+    <row r="32" spans="1:29" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="89"/>
+      <c r="B32" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="109">
-        <f>SUM(C5,C11,C15,C26)</f>
-        <v>78</v>
-      </c>
-      <c r="D28" s="109" t="str">
-        <f>IF(SUM(J28:AC28)=0," ",SUM(J28:AC28))</f>
+      <c r="C32" s="109">
+        <f>SUM(C5,C11,C15,C30)</f>
+        <v>204</v>
+      </c>
+      <c r="D32" s="109" t="str">
+        <f>IF(SUM(J32:AC32)=0," ",SUM(J32:AC32))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="112">
-        <f t="shared" ref="J28:AC28" si="3">SUM(J5:J27)</f>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="111"/>
+      <c r="J32" s="112">
+        <f t="shared" ref="J32:AC32" si="3">SUM(J5:J31)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="109">
+      <c r="K32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L28" s="113">
+      <c r="L32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M28" s="113">
+      <c r="M32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N28" s="113">
+      <c r="N32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O28" s="113">
+      <c r="O32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P28" s="109">
+      <c r="P32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="113">
+      <c r="Q32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R28" s="109">
+      <c r="R32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S28" s="113">
+      <c r="S32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T28" s="113">
+      <c r="T32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U28" s="109">
+      <c r="U32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V28" s="113">
+      <c r="V32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W28" s="109">
+      <c r="W32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X28" s="113">
+      <c r="X32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Y28" s="113">
+      <c r="Y32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="109">
+      <c r="Z32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="113">
+      <c r="AA32" s="113">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="109">
+      <c r="AB32" s="109">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="114">
+      <c r="AC32" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="115"/>
-      <c r="B29" s="169"/>
-      <c r="C29" s="169"/>
-      <c r="D29" s="169"/>
-      <c r="E29" s="169"/>
-      <c r="F29" s="169"/>
-      <c r="G29" s="169"/>
-      <c r="H29" s="169"/>
-      <c r="I29" s="169"/>
-    </row>
-    <row r="30" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="118"/>
-      <c r="B30" s="15" t="s">
+    <row r="33" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="115"/>
+      <c r="B33" s="167"/>
+      <c r="C33" s="167"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
+      <c r="G33" s="167"/>
+      <c r="H33" s="167"/>
+      <c r="I33" s="167"/>
+    </row>
+    <row r="34" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="118"/>
+      <c r="B34" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="167"/>
-      <c r="K30" s="168"/>
-      <c r="L30" s="168"/>
-      <c r="M30" s="168"/>
-      <c r="N30" s="168"/>
-      <c r="O30" s="168"/>
-      <c r="P30" s="168"/>
-      <c r="Q30" s="168"/>
-      <c r="R30" s="168"/>
-      <c r="S30" s="168"/>
-      <c r="T30" s="168"/>
-      <c r="U30" s="168"/>
-      <c r="V30" s="168"/>
-      <c r="W30" s="168"/>
-      <c r="X30" s="168"/>
-      <c r="Y30" s="168"/>
-      <c r="Z30" s="168"/>
-      <c r="AA30" s="168"/>
-      <c r="AB30" s="168"/>
-      <c r="AC30" s="168"/>
-    </row>
-    <row r="31" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="165"/>
-      <c r="B31" s="14" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="165"/>
+      <c r="K34" s="166"/>
+      <c r="L34" s="166"/>
+      <c r="M34" s="166"/>
+      <c r="N34" s="166"/>
+      <c r="O34" s="166"/>
+      <c r="P34" s="166"/>
+      <c r="Q34" s="166"/>
+      <c r="R34" s="166"/>
+      <c r="S34" s="166"/>
+      <c r="T34" s="166"/>
+      <c r="U34" s="166"/>
+      <c r="V34" s="166"/>
+      <c r="W34" s="166"/>
+      <c r="X34" s="166"/>
+      <c r="Y34" s="166"/>
+      <c r="Z34" s="166"/>
+      <c r="AA34" s="166"/>
+      <c r="AB34" s="166"/>
+      <c r="AC34" s="166"/>
+    </row>
+    <row r="35" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="163"/>
+      <c r="B35" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="166"/>
-      <c r="K31" s="166"/>
-      <c r="L31" s="166"/>
-      <c r="M31" s="166"/>
-      <c r="N31" s="166"/>
-      <c r="O31" s="166"/>
-      <c r="P31" s="166"/>
-      <c r="Q31" s="166"/>
-      <c r="R31" s="166"/>
-      <c r="S31" s="166"/>
-      <c r="T31" s="166"/>
-      <c r="U31" s="166"/>
-      <c r="V31" s="166"/>
-      <c r="W31" s="166"/>
-      <c r="X31" s="166"/>
-      <c r="Y31" s="166"/>
-      <c r="Z31" s="166"/>
-      <c r="AA31" s="166"/>
-      <c r="AB31" s="166"/>
-      <c r="AC31" s="166"/>
-    </row>
-    <row r="32" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="166"/>
-      <c r="K32" s="166"/>
-      <c r="L32" s="166"/>
-      <c r="M32" s="166"/>
-      <c r="N32" s="166"/>
-      <c r="O32" s="166"/>
-      <c r="P32" s="166"/>
-      <c r="Q32" s="166"/>
-      <c r="R32" s="166"/>
-      <c r="S32" s="166"/>
-      <c r="T32" s="166"/>
-      <c r="U32" s="166"/>
-      <c r="V32" s="166"/>
-      <c r="W32" s="166"/>
-      <c r="X32" s="166"/>
-      <c r="Y32" s="166"/>
-      <c r="Z32" s="166"/>
-      <c r="AA32" s="166"/>
-      <c r="AB32" s="166"/>
-      <c r="AC32" s="166"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="18"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="18"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="18"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="20"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="19"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="164"/>
+      <c r="K35" s="164"/>
+      <c r="L35" s="164"/>
+      <c r="M35" s="164"/>
+      <c r="N35" s="164"/>
+      <c r="O35" s="164"/>
+      <c r="P35" s="164"/>
+      <c r="Q35" s="164"/>
+      <c r="R35" s="164"/>
+      <c r="S35" s="164"/>
+      <c r="T35" s="164"/>
+      <c r="U35" s="164"/>
+      <c r="V35" s="164"/>
+      <c r="W35" s="164"/>
+      <c r="X35" s="164"/>
+      <c r="Y35" s="164"/>
+      <c r="Z35" s="164"/>
+      <c r="AA35" s="164"/>
+      <c r="AB35" s="164"/>
+      <c r="AC35" s="164"/>
+    </row>
+    <row r="36" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="164"/>
+      <c r="K36" s="164"/>
+      <c r="L36" s="164"/>
+      <c r="M36" s="164"/>
+      <c r="N36" s="164"/>
+      <c r="O36" s="164"/>
+      <c r="P36" s="164"/>
+      <c r="Q36" s="164"/>
+      <c r="R36" s="164"/>
+      <c r="S36" s="164"/>
+      <c r="T36" s="164"/>
+      <c r="U36" s="164"/>
+      <c r="V36" s="164"/>
+      <c r="W36" s="164"/>
+      <c r="X36" s="164"/>
+      <c r="Y36" s="164"/>
+      <c r="Z36" s="164"/>
+      <c r="AA36" s="164"/>
+      <c r="AB36" s="164"/>
+      <c r="AC36" s="164"/>
+    </row>
+    <row r="37" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="18"/>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+      <c r="B38" s="18"/>
       <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="18"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="J31:AC32"/>
-    <mergeCell ref="J30:AC30"/>
-    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="J35:AC36"/>
+    <mergeCell ref="J34:AC34"/>
+    <mergeCell ref="B33:I33"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="T3:X3"/>
     <mergeCell ref="Y3:AC3"/>
@@ -4326,7 +4547,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:B30"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4339,21 +4560,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="177"/>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
+      <c r="A1" s="175"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="175"/>
+      <c r="N1" s="175"/>
+      <c r="O1" s="175"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -4392,7 +4613,7 @@
         <v>42702</v>
       </c>
       <c r="C4" s="5">
-        <f>'IPA Zeitplanung'!J28</f>
+        <f>'IPA Zeitplanung'!J32</f>
         <v>0</v>
       </c>
     </row>
@@ -4405,7 +4626,7 @@
         <v>42703</v>
       </c>
       <c r="C5" s="5">
-        <f>'IPA Zeitplanung'!K28</f>
+        <f>'IPA Zeitplanung'!K32</f>
         <v>0</v>
       </c>
     </row>
@@ -4418,7 +4639,7 @@
         <v>42704</v>
       </c>
       <c r="C6" s="5">
-        <f>'IPA Zeitplanung'!L28</f>
+        <f>'IPA Zeitplanung'!L32</f>
         <v>0</v>
       </c>
     </row>
@@ -4431,7 +4652,7 @@
         <v>42705</v>
       </c>
       <c r="C7" s="5">
-        <f>'IPA Zeitplanung'!M28</f>
+        <f>'IPA Zeitplanung'!M32</f>
         <v>0</v>
       </c>
     </row>
@@ -4444,7 +4665,7 @@
         <v>42706</v>
       </c>
       <c r="C8" s="5">
-        <f>'IPA Zeitplanung'!N28</f>
+        <f>'IPA Zeitplanung'!N32</f>
         <v>0</v>
       </c>
     </row>
@@ -4457,7 +4678,7 @@
         <v>42709</v>
       </c>
       <c r="C9" s="5">
-        <f>'IPA Zeitplanung'!O28</f>
+        <f>'IPA Zeitplanung'!O32</f>
         <v>0</v>
       </c>
     </row>
@@ -4470,7 +4691,7 @@
         <v>42710</v>
       </c>
       <c r="C10" s="5">
-        <f>'IPA Zeitplanung'!P28</f>
+        <f>'IPA Zeitplanung'!P32</f>
         <v>0</v>
       </c>
     </row>
@@ -4483,7 +4704,7 @@
         <v>42711</v>
       </c>
       <c r="C11" s="5">
-        <f>'IPA Zeitplanung'!Q28</f>
+        <f>'IPA Zeitplanung'!Q32</f>
         <v>0</v>
       </c>
     </row>
@@ -4496,7 +4717,7 @@
         <v>42712</v>
       </c>
       <c r="C12" s="5">
-        <f>'IPA Zeitplanung'!R28</f>
+        <f>'IPA Zeitplanung'!R32</f>
         <v>0</v>
       </c>
     </row>
@@ -4509,7 +4730,7 @@
         <v>42713</v>
       </c>
       <c r="C13" s="5">
-        <f>'IPA Zeitplanung'!S28</f>
+        <f>'IPA Zeitplanung'!S32</f>
         <v>0</v>
       </c>
     </row>
@@ -4522,7 +4743,7 @@
         <v>42716</v>
       </c>
       <c r="C14" s="5">
-        <f>'IPA Zeitplanung'!T28</f>
+        <f>'IPA Zeitplanung'!T32</f>
         <v>0</v>
       </c>
     </row>
@@ -4535,7 +4756,7 @@
         <v>42717</v>
       </c>
       <c r="C15" s="5">
-        <f>'IPA Zeitplanung'!U28</f>
+        <f>'IPA Zeitplanung'!U32</f>
         <v>0</v>
       </c>
     </row>
@@ -4548,7 +4769,7 @@
         <v>42718</v>
       </c>
       <c r="C16" s="5">
-        <f>'IPA Zeitplanung'!V28</f>
+        <f>'IPA Zeitplanung'!V32</f>
         <v>0</v>
       </c>
     </row>
@@ -4561,7 +4782,7 @@
         <v>42719</v>
       </c>
       <c r="C17" s="5">
-        <f>'IPA Zeitplanung'!W28</f>
+        <f>'IPA Zeitplanung'!W32</f>
         <v>0</v>
       </c>
     </row>
@@ -4574,7 +4795,7 @@
         <v>42720</v>
       </c>
       <c r="C18" s="5">
-        <f>'IPA Zeitplanung'!X28</f>
+        <f>'IPA Zeitplanung'!X32</f>
         <v>0</v>
       </c>
     </row>
@@ -4587,7 +4808,7 @@
         <v>42723</v>
       </c>
       <c r="C19" s="5">
-        <f>'IPA Zeitplanung'!Y28</f>
+        <f>'IPA Zeitplanung'!Y32</f>
         <v>0</v>
       </c>
     </row>
@@ -4600,7 +4821,7 @@
         <v>42724</v>
       </c>
       <c r="C20" s="5">
-        <f>'IPA Zeitplanung'!Z28</f>
+        <f>'IPA Zeitplanung'!Z32</f>
         <v>0</v>
       </c>
     </row>
@@ -4613,7 +4834,7 @@
         <v>42725</v>
       </c>
       <c r="C21" s="5">
-        <f>'IPA Zeitplanung'!AA28</f>
+        <f>'IPA Zeitplanung'!AA32</f>
         <v>0</v>
       </c>
     </row>
@@ -4626,7 +4847,7 @@
         <v>42726</v>
       </c>
       <c r="C22" s="5">
-        <f>'IPA Zeitplanung'!AB28</f>
+        <f>'IPA Zeitplanung'!AB32</f>
         <v>0</v>
       </c>
     </row>
@@ -4639,7 +4860,7 @@
         <v>42727</v>
       </c>
       <c r="C23" s="5">
-        <f>'IPA Zeitplanung'!AC28</f>
+        <f>'IPA Zeitplanung'!AC32</f>
         <v>0</v>
       </c>
     </row>
@@ -4659,10 +4880,10 @@
     <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="178" t="s">
+      <c r="A27" s="176" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="179"/>
+      <c r="B27" s="177"/>
       <c r="C27" s="4" t="s">
         <v>25</v>
       </c>
@@ -4671,13 +4892,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="175" t="s">
+      <c r="A28" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="176"/>
+      <c r="B28" s="174"/>
       <c r="C28" s="5">
         <f>'IPA Zeitplanung'!C5</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D28" s="5">
         <f>'IPA Zeitplanung'!D5</f>
@@ -4685,27 +4906,27 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="180" t="s">
+      <c r="A29" s="178" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="181"/>
+      <c r="B29" s="179"/>
       <c r="C29" s="5">
         <f>'IPA Zeitplanung'!C11</f>
         <v>1</v>
       </c>
       <c r="D29" s="5">
         <f>'IPA Zeitplanung'!D11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="175" t="s">
+      <c r="A30" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="176"/>
+      <c r="B30" s="174"/>
       <c r="C30" s="5">
         <f>'IPA Zeitplanung'!C15</f>
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="D30" s="5">
         <f>'IPA Zeitplanung'!D15</f>
@@ -4713,10 +4934,10 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="180" t="s">
+      <c r="A31" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="181"/>
+      <c r="B31" s="179"/>
       <c r="C31" s="5" t="e">
         <f>'IPA Zeitplanung'!#REF!</f>
         <v>#REF!</v>
@@ -4727,24 +4948,24 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="175" t="s">
+      <c r="A32" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="176"/>
+      <c r="B32" s="174"/>
       <c r="C32" s="5">
-        <f>'IPA Zeitplanung'!C26</f>
-        <v>26</v>
+        <f>'IPA Zeitplanung'!C30</f>
+        <v>34</v>
       </c>
       <c r="D32" s="5">
-        <f>SUM('IPA Zeitplanung'!D26)</f>
+        <f>SUM('IPA Zeitplanung'!D30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="175" t="s">
+      <c r="A33" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="176"/>
+      <c r="B33" s="174"/>
       <c r="C33" s="5" t="e">
         <f>'IPA Zeitplanung'!#REF!</f>
         <v>#REF!</v>

</xml_diff>